<commit_message>
Adding code to repo
</commit_message>
<xml_diff>
--- a/src/TestData/Data.xlsx
+++ b/src/TestData/Data.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="ObjectR" sheetId="1" r:id="rId1"/>
     <sheet name="TestD" sheetId="2" r:id="rId2"/>
+    <sheet name="ConfigurationD" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>Locator_Type</t>
   </si>
@@ -35,18 +36,6 @@
     <t>Data_Value</t>
   </si>
   <si>
-    <t>Flight_From</t>
-  </si>
-  <si>
-    <t>DEL</t>
-  </si>
-  <si>
-    <t>Flight_to</t>
-  </si>
-  <si>
-    <t>MUM</t>
-  </si>
-  <si>
     <t>btn_cookies</t>
   </si>
   <si>
@@ -123,13 +112,43 @@
   </si>
   <si>
     <t>//div[@class='FPdoLc VlcLAe']//input[@value='Google Search']</t>
+  </si>
+  <si>
+    <t>Nummer</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>as00360417@techmahindra.com</t>
+  </si>
+  <si>
+    <t>Data_Required</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insurance </t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Capacity_20</t>
+  </si>
+  <si>
+    <t>Capacity_32</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,14 +168,6 @@
       <sz val="10"/>
       <color rgb="FF303336"/>
       <name val="Inherit"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -191,11 +202,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -501,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -531,149 +542,179 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D2"/>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D3"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>21</v>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>17</v>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>22</v>
+      <c r="C8" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>35</v>
+    <row r="16" spans="1:5">
+      <c r="A16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -687,37 +728,92 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1">
+        <v>52766579</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>37</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>